<commit_message>
excel tareas y BBDD
</commit_message>
<xml_diff>
--- a/ludyfest.xlsx
+++ b/ludyfest.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Asistencia</t>
   </si>
@@ -69,22 +69,40 @@
     <t>ruta de login, modelo y controlador</t>
   </si>
   <si>
+    <t>alejandro</t>
+  </si>
+  <si>
     <t>Registro de usuarios</t>
   </si>
   <si>
     <t>ruta de registro de usuario, modelo y controlador</t>
   </si>
   <si>
-    <t>home</t>
+    <t>jonatan</t>
+  </si>
+  <si>
+    <t>home, crear ruta, cargarla, maquetar</t>
+  </si>
+  <si>
+    <t>Angel</t>
   </si>
   <si>
     <t>ruta de eventos getAll para obtener todos los eventos, controlador, modelo, query</t>
   </si>
   <si>
+    <t>pati</t>
+  </si>
+  <si>
     <t>listado de eventos publico</t>
   </si>
   <si>
+    <t>fabrizo</t>
+  </si>
+  <si>
     <t>ruta de eventos getById para obtener un evento,controlador, query</t>
+  </si>
+  <si>
+    <t>Edward</t>
   </si>
   <si>
     <t>filtro de eventos</t>
@@ -133,6 +151,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10.0"/>
@@ -200,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -226,6 +247,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -655,87 +679,132 @@
       <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="9">
+        <v>45861.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="9">
+        <v>45862.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45861.0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="9">
+        <v>45863.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45861.0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="9">
+        <v>45864.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="H6" s="9">
+        <v>45865.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="H7" s="9">
+        <v>45866.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="H8" s="9">
+        <v>45867.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lista de tareas actualizada
</commit_message>
<xml_diff>
--- a/ludyfest.xlsx
+++ b/ludyfest.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t>Asistencia</t>
   </si>
@@ -111,6 +111,9 @@
     <t>ruta de eventos delete para obtener un evento,controlador, query</t>
   </si>
   <si>
+    <t>Anghel</t>
+  </si>
+  <si>
     <t>vista de evento concreto, componente, ruta</t>
   </si>
   <si>
@@ -126,7 +129,7 @@
     <t>ruta de eventos apuntarse a un evento para obtener un evento,controlador, query</t>
   </si>
   <si>
-    <t>listado de eventos para administrador, ruta, componente, interfaz</t>
+    <t>listado de eventos para administrador, ruta, componente, interfaz, boton actualizar y borrar</t>
   </si>
   <si>
     <t>patricia</t>
@@ -138,7 +141,7 @@
     <t>CRUD de eventos administrados boton borrar, actualizar, crear nuevo</t>
   </si>
   <si>
-    <t>seguridad token y hash password</t>
+    <t>seguridad  hash password</t>
   </si>
   <si>
     <t>formulario de creacion de evento, componente, ruta y enviar al servicio</t>
@@ -157,6 +160,33 @@
   </si>
   <si>
     <t>definición de rutas, tanto publicas como privadas. (Tarea continua)</t>
+  </si>
+  <si>
+    <t>getID de usuarios</t>
+  </si>
+  <si>
+    <t>conectar el events publico con el back y traer todos los eventos, servicio, getAll front y conectar la ruta de back</t>
+  </si>
+  <si>
+    <t>fabrizio</t>
+  </si>
+  <si>
+    <t>borrar usuarios</t>
+  </si>
+  <si>
+    <t>listado de eventos de admistrador tambien getAll</t>
+  </si>
+  <si>
+    <t>creacion token</t>
+  </si>
+  <si>
+    <t>administracion de listado de usuario</t>
+  </si>
+  <si>
+    <t>ruta para registrar un evento</t>
+  </si>
+  <si>
+    <t>juanjo</t>
   </si>
 </sst>
 </file>
@@ -239,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -249,10 +279,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -271,6 +301,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -532,6 +565,9 @@
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
@@ -540,6 +576,9 @@
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
@@ -548,6 +587,9 @@
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -556,6 +598,9 @@
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
@@ -564,6 +609,9 @@
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -572,12 +620,18 @@
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -665,7 +719,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="59.75"/>
+    <col customWidth="1" min="1" max="1" width="82.5"/>
     <col customWidth="1" min="6" max="6" width="65.13"/>
   </cols>
   <sheetData>
@@ -754,13 +808,13 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="11">
         <v>45861.0</v>
       </c>
       <c r="F5" s="10" t="s">
@@ -780,33 +834,45 @@
       <c r="F6" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H6" s="9">
-        <v>45861.0</v>
+        <v>45863.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="9">
         <v>45862.0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="H7" s="9">
-        <v>45861.0</v>
+        <v>45863.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45863.0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H8" s="9">
         <v>45861.0</v>
@@ -814,46 +880,55 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="9">
         <v>45862.0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="9">
         <v>45862.0</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>44</v>
+      <c r="F11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="9">
+        <v>45862.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>20</v>
@@ -864,7 +939,61 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="9">
+        <v>45863.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="9">
+        <v>45863.0</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="9">
+        <v>45863.0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="9">
+        <v>45863.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>